<commit_message>
file in static folder
</commit_message>
<xml_diff>
--- a/donefiles/leemoispace@gmail.com.xlsx
+++ b/donefiles/leemoispace@gmail.com.xlsx
@@ -381,16 +381,16 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2333</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>233</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>86</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>